<commit_message>
check type import square warehouse
</commit_message>
<xml_diff>
--- a/td_template_import/square_warehouses.xlsx
+++ b/td_template_import/square_warehouses.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$38</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,9 +61,6 @@
     <t>MB58</t>
   </si>
   <si>
-    <t>Màng bóng 58</t>
-  </si>
-  <si>
     <t>MB58-15A</t>
   </si>
   <si>
@@ -118,9 +118,6 @@
     <t>MBN69</t>
   </si>
   <si>
-    <t>Màng bóng nước khổ 69 loại 12 mic</t>
-  </si>
-  <si>
     <t>MM101-16B</t>
   </si>
   <si>
@@ -172,33 +169,18 @@
     <t>MMN44.5</t>
   </si>
   <si>
-    <t>Màng mờ nước khổ 44.5 loại 15 mic</t>
-  </si>
-  <si>
     <t>MMN54</t>
   </si>
   <si>
-    <t>Màng mờ nước khổ 54 loại 15 mic</t>
-  </si>
-  <si>
     <t>MMN64.5</t>
   </si>
   <si>
-    <t>Màng mờ nước khổ 64.5 loại 15 mic</t>
-  </si>
-  <si>
     <t>MMN78</t>
   </si>
   <si>
-    <t>Màng mờ nước khổ 78 loại 12 mic</t>
-  </si>
-  <si>
     <t>MMN89</t>
   </si>
   <si>
-    <t>Màng mờ nước khổ 89 loại 12 mic</t>
-  </si>
-  <si>
     <t>MMT39.5</t>
   </si>
   <si>
@@ -257,6 +239,27 @@
   </si>
   <si>
     <t>Màng Metalai bạc khổ 87.5</t>
+  </si>
+  <si>
+    <t>Màng bóng nước khổ 69</t>
+  </si>
+  <si>
+    <t>Màng mờ nước khổ 44.5</t>
+  </si>
+  <si>
+    <t>Màng mờ nước khổ 54</t>
+  </si>
+  <si>
+    <t>Màng mờ nước khổ 64.5</t>
+  </si>
+  <si>
+    <t>Màng mờ nước khổ 78</t>
+  </si>
+  <si>
+    <t>Màng mờ nước khổ 89</t>
+  </si>
+  <si>
+    <t>Màng bóng khổ 58</t>
   </si>
 </sst>
 </file>
@@ -620,13 +623,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -690,7 +694,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -701,10 +705,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -715,10 +719,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -729,10 +733,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -743,10 +747,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -757,10 +761,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -771,10 +775,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -785,10 +789,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
@@ -799,10 +803,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -813,10 +817,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -827,10 +831,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -841,10 +845,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
@@ -855,10 +859,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
@@ -869,10 +873,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
@@ -883,10 +887,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -897,10 +901,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>6</v>
@@ -911,10 +915,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>6</v>
@@ -925,10 +929,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>6</v>
@@ -939,10 +943,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>6</v>
@@ -953,10 +957,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -967,10 +971,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
@@ -981,10 +985,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>6</v>
@@ -995,10 +999,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
@@ -1009,10 +1013,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -1023,10 +1027,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
@@ -1037,10 +1041,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -1051,10 +1055,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>6</v>
@@ -1065,10 +1069,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -1079,10 +1083,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
@@ -1093,10 +1097,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>6</v>
@@ -1107,10 +1111,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
@@ -1121,10 +1125,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
@@ -1135,10 +1139,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>6</v>
@@ -1149,10 +1153,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>6</v>
@@ -1162,6 +1166,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D38"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>